<commit_message>
v2 template and adjust generate report
</commit_message>
<xml_diff>
--- a/public/templates/rictu_report_template.xlsx
+++ b/public/templates/rictu_report_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laravel\dilg4a_portal-main\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laravel\dilg4a_portal\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7E9184-EE57-4C11-AB19-2A9E84128EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EDE0EB-EFD4-42E6-A7D1-3E26CB98F9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -588,6 +588,36 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -611,36 +641,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -981,7 +981,7 @@
   <dimension ref="A1:M195"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1019,50 +1019,50 @@
     <row r="2" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
       <c r="H2" s="11"/>
       <c r="I2"/>
       <c r="J2"/>
-      <c r="K2" s="47" t="s">
+      <c r="K2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="48"/>
-      <c r="M2" s="49"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="59"/>
     </row>
     <row r="3" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
       <c r="H3" s="11"/>
       <c r="I3"/>
       <c r="J3"/>
-      <c r="K3" s="50" t="s">
+      <c r="K3" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="51"/>
-      <c r="M3" s="52"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="62"/>
     </row>
     <row r="4" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4"/>
       <c r="B4"/>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4" s="3" t="s">
@@ -1078,12 +1078,12 @@
     <row r="5" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5"/>
       <c r="B5"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5" s="4" t="s">
@@ -1110,70 +1110,70 @@
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="56"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
     </row>
     <row r="8" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="60"/>
-      <c r="E8" s="57" t="s">
+      <c r="D8" s="52"/>
+      <c r="E8" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="F8" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="57" t="s">
+      <c r="G8" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="57" t="s">
+      <c r="H8" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="59" t="s">
+      <c r="I8" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="60"/>
-      <c r="K8" s="59" t="s">
+      <c r="J8" s="52"/>
+      <c r="K8" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="60"/>
-      <c r="M8" s="61" t="s">
+      <c r="L8" s="52"/>
+      <c r="M8" s="53" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="58"/>
-      <c r="B9" s="58"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
       <c r="I9" s="12" t="s">
         <v>6</v>
       </c>
@@ -1186,7 +1186,7 @@
       <c r="L9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="62"/>
+      <c r="M9" s="54"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="26"/>
@@ -1850,6 +1850,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="C4:H5"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:M7"/>
     <mergeCell ref="H8:H9"/>
@@ -1862,11 +1867,6 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="C4:H5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.15748031496062992" bottom="0.23622047244094491" header="0.15748031496062992" footer="0.27559055118110237"/>
   <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
adjust total process time on template
</commit_message>
<xml_diff>
--- a/public/templates/rictu_report_template.xlsx
+++ b/public/templates/rictu_report_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laravel\dilg4a_portal\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCE20BE-729E-4B89-BFD3-0572D7CC9D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40F76D1-DC8E-4AAA-AA17-1982BADCCCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -506,9 +506,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -551,13 +548,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -579,11 +572,14 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -978,24 +974,24 @@
   <dimension ref="A1:M195"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.08984375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" style="19" customWidth="1"/>
-    <col min="4" max="4" width="6.90625" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.08984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="6.90625" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.08984375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="18.6328125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="18.6328125" style="15" customWidth="1"/>
     <col min="7" max="7" width="53.54296875" style="14" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" style="16" customWidth="1"/>
-    <col min="9" max="9" width="9.90625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" style="15" customWidth="1"/>
+    <col min="9" max="9" width="9.90625" style="17" customWidth="1"/>
     <col min="10" max="10" width="10.1796875" style="13" customWidth="1"/>
-    <col min="11" max="11" width="14.6328125" style="17" customWidth="1"/>
-    <col min="12" max="12" width="6.90625" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.90625" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6328125" style="16" customWidth="1"/>
+    <col min="12" max="12" width="6.90625" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.90625" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
@@ -1016,50 +1012,50 @@
     <row r="2" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
       <c r="H2" s="11"/>
       <c r="I2"/>
       <c r="J2"/>
-      <c r="K2" s="56" t="s">
+      <c r="K2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="57"/>
-      <c r="M2" s="58"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="56"/>
     </row>
     <row r="3" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
       <c r="H3" s="11"/>
       <c r="I3"/>
       <c r="J3"/>
-      <c r="K3" s="59" t="s">
+      <c r="K3" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="60"/>
-      <c r="M3" s="61"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="59"/>
     </row>
     <row r="4" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4"/>
       <c r="B4"/>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4" s="3" t="s">
@@ -1075,12 +1071,12 @@
     <row r="5" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5"/>
       <c r="B5"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5" s="4" t="s">
@@ -1089,7 +1085,7 @@
       <c r="L5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="44"/>
+      <c r="M5" s="40"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6"/>
@@ -1107,70 +1103,70 @@
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
     </row>
     <row r="8" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="48" t="s">
+      <c r="D8" s="49"/>
+      <c r="E8" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="48" t="s">
+      <c r="F8" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="48" t="s">
+      <c r="G8" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="48" t="s">
+      <c r="H8" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="51"/>
-      <c r="K8" s="50" t="s">
+      <c r="J8" s="49"/>
+      <c r="K8" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="51"/>
-      <c r="M8" s="52" t="s">
+      <c r="L8" s="49"/>
+      <c r="M8" s="50" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="49"/>
-      <c r="B9" s="49"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
       <c r="I9" s="12" t="s">
         <v>6</v>
       </c>
@@ -1183,667 +1179,662 @@
       <c r="L9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="53"/>
+      <c r="M9" s="51"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="29"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="28"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="26"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="29"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="28"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="26"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="29"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="28"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="29"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="28"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="26"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="29"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="28"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="29"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="28"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="26"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="29"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="28"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="29"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="28"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="26"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="29"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="28"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="29"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="28"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="26"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="29"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="28"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="26"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="29"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="28"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="26"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="29"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="28"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="26"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="29"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="28"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="26"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="29"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="28"/>
       <c r="J24" s="2"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="26"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="29"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="28"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="26"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="29"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="28"/>
       <c r="J26" s="2"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="26"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="29"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="28"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="26"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="29"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="28"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="26"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="26"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="29"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="28"/>
       <c r="J29" s="2"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-    </row>
-    <row r="30" spans="1:13" s="38" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A30" s="37"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="37"/>
-      <c r="L30" s="37"/>
-      <c r="M30" s="36"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+    </row>
+    <row r="30" spans="1:13" s="35" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="33"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="31"/>
+      <c r="C31" s="30"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="27"/>
+      <c r="E31" s="26"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="27"/>
+      <c r="G31" s="26"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="29"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="28"/>
       <c r="L31" s="2"/>
-      <c r="M31" s="33"/>
+      <c r="M31" s="26"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="31"/>
+      <c r="C32" s="30"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="27"/>
+      <c r="E32" s="26"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="27"/>
+      <c r="G32" s="26"/>
       <c r="H32" s="2"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="29"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="28"/>
       <c r="L32" s="2"/>
-      <c r="M32" s="33"/>
+      <c r="M32" s="26"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="31"/>
+      <c r="C33" s="30"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="27"/>
+      <c r="E33" s="26"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="27"/>
+      <c r="G33" s="26"/>
       <c r="H33" s="2"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="29"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="28"/>
       <c r="L33" s="2"/>
-      <c r="M33" s="33"/>
+      <c r="M33" s="26"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="31"/>
+      <c r="C34" s="30"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="27"/>
+      <c r="E34" s="26"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="27"/>
+      <c r="G34" s="26"/>
       <c r="H34" s="2"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="29"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="28"/>
       <c r="L34" s="2"/>
-      <c r="M34" s="33"/>
+      <c r="M34" s="26"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="31"/>
+      <c r="C35" s="30"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="27"/>
+      <c r="E35" s="26"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="27"/>
+      <c r="G35" s="26"/>
       <c r="H35" s="2"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="29"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="28"/>
       <c r="L35" s="2"/>
-      <c r="M35" s="33"/>
+      <c r="M35" s="26"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="34"/>
+      <c r="G36" s="32"/>
       <c r="H36" s="2"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="29"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="28"/>
       <c r="L36" s="2"/>
-      <c r="M36" s="33"/>
+      <c r="M36" s="26"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="34"/>
+      <c r="G37" s="32"/>
       <c r="H37" s="2"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="29"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="28"/>
       <c r="L37" s="2"/>
-      <c r="M37" s="33"/>
+      <c r="M37" s="26"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="34"/>
+      <c r="G38" s="32"/>
       <c r="H38" s="2"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="29"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="28"/>
       <c r="L38" s="2"/>
-      <c r="M38" s="33"/>
+      <c r="M38" s="26"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="34"/>
+      <c r="G39" s="32"/>
       <c r="H39" s="2"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="29"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="28"/>
       <c r="L39" s="2"/>
-      <c r="M39" s="33"/>
+      <c r="M39" s="26"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
       <c r="F40" s="2"/>
-      <c r="G40" s="34"/>
+      <c r="G40" s="32"/>
       <c r="H40" s="2"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="29"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="28"/>
       <c r="L40" s="2"/>
-      <c r="M40" s="33"/>
+      <c r="M40" s="26"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="34"/>
+      <c r="G41" s="32"/>
       <c r="H41" s="2"/>
-      <c r="I41" s="32"/>
-      <c r="J41" s="30"/>
-      <c r="K41" s="29"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="28"/>
       <c r="L41" s="2"/>
-      <c r="M41" s="33"/>
+      <c r="M41" s="26"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="34"/>
+      <c r="G42" s="32"/>
       <c r="H42" s="2"/>
-      <c r="I42" s="32"/>
-      <c r="J42" s="30"/>
-      <c r="K42" s="29"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="28"/>
       <c r="L42" s="2"/>
-      <c r="M42" s="33"/>
+      <c r="M42" s="26"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
-      <c r="C43" s="31"/>
+      <c r="C43" s="30"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="27"/>
+      <c r="E43" s="26"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="27"/>
+      <c r="G43" s="26"/>
       <c r="H43" s="2"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="30"/>
-      <c r="K43" s="29"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="28"/>
       <c r="L43" s="2"/>
-      <c r="M43" s="33"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A44" s="41"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
-      <c r="K44" s="35"/>
-      <c r="L44" s="35"/>
-      <c r="M44" s="35"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-      <c r="K45" s="13"/>
-      <c r="L45" s="13"/>
-      <c r="M45" s="13"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
-      <c r="M46" s="13"/>
-    </row>
-    <row r="47" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="K47" s="13"/>
-      <c r="L47" s="13"/>
-      <c r="M47" s="13"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
-      <c r="K48" s="13"/>
-      <c r="L48" s="13"/>
-      <c r="M48" s="13"/>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B49" s="13"/>
-      <c r="C49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-      <c r="K49" s="13"/>
-      <c r="L49" s="13"/>
-      <c r="M49" s="13"/>
+      <c r="M43" s="26"/>
+    </row>
+    <row r="44" spans="1:13" s="15" customFormat="1" ht="10.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="38"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="38"/>
+      <c r="K44" s="38"/>
+      <c r="L44" s="38"/>
+      <c r="M44" s="41"/>
+    </row>
+    <row r="45" spans="1:13" s="15" customFormat="1" ht="10.5" x14ac:dyDescent="0.35">
+      <c r="M45" s="14"/>
+    </row>
+    <row r="46" spans="1:13" s="15" customFormat="1" ht="10.5" x14ac:dyDescent="0.35">
+      <c r="M46" s="14"/>
+    </row>
+    <row r="47" spans="1:13" s="15" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M47" s="14"/>
+    </row>
+    <row r="48" spans="1:13" s="15" customFormat="1" ht="10.5" x14ac:dyDescent="0.35">
+      <c r="M48" s="14"/>
+    </row>
+    <row r="49" spans="3:13" s="15" customFormat="1" ht="10.5" x14ac:dyDescent="0.35">
+      <c r="M49" s="14"/>
+    </row>
+    <row r="50" spans="3:13" s="15" customFormat="1" ht="10.5" x14ac:dyDescent="0.35">
+      <c r="C50" s="18"/>
+      <c r="E50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="I50" s="16"/>
+      <c r="K50" s="16"/>
+      <c r="M50" s="14"/>
+    </row>
+    <row r="51" spans="3:13" s="15" customFormat="1" ht="10.5" x14ac:dyDescent="0.35">
+      <c r="C51" s="18"/>
+      <c r="E51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="I51" s="16"/>
+      <c r="K51" s="16"/>
+      <c r="M51" s="14"/>
+    </row>
+    <row r="52" spans="3:13" s="15" customFormat="1" ht="10.5" x14ac:dyDescent="0.35">
+      <c r="C52" s="18"/>
+      <c r="E52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="I52" s="16"/>
+      <c r="K52" s="16"/>
+      <c r="M52" s="14"/>
+    </row>
+    <row r="53" spans="3:13" s="15" customFormat="1" ht="10.5" x14ac:dyDescent="0.35">
+      <c r="C53" s="18"/>
+      <c r="E53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="I53" s="16"/>
+      <c r="K53" s="16"/>
+      <c r="M53" s="14"/>
+    </row>
+    <row r="54" spans="3:13" s="15" customFormat="1" ht="10.5" x14ac:dyDescent="0.35">
+      <c r="C54" s="18"/>
+      <c r="E54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="I54" s="16"/>
+      <c r="K54" s="16"/>
+      <c r="M54" s="14"/>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A191" s="40"/>
-      <c r="B191" s="21"/>
-      <c r="C191" s="21"/>
-      <c r="D191" s="25"/>
-      <c r="E191" s="20"/>
-      <c r="F191" s="20"/>
-      <c r="G191" s="25"/>
-      <c r="H191" s="20"/>
-      <c r="I191" s="20"/>
-      <c r="J191" s="20"/>
-      <c r="K191" s="21"/>
-      <c r="L191" s="21"/>
-      <c r="M191" s="21"/>
+      <c r="A191" s="37"/>
+      <c r="B191" s="20"/>
+      <c r="C191" s="24"/>
+      <c r="D191" s="24"/>
+      <c r="E191" s="19"/>
+      <c r="F191" s="19"/>
+      <c r="G191" s="24"/>
+      <c r="H191" s="19"/>
+      <c r="I191" s="19"/>
+      <c r="J191" s="19"/>
+      <c r="K191" s="20"/>
+      <c r="L191" s="20"/>
+      <c r="M191" s="42"/>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A192" s="42"/>
-      <c r="B192" s="21"/>
-      <c r="C192" s="21"/>
-      <c r="D192" s="25"/>
-      <c r="E192" s="22"/>
-      <c r="F192" s="22"/>
-      <c r="G192" s="25"/>
-      <c r="H192" s="22"/>
-      <c r="I192" s="22"/>
-      <c r="J192" s="22"/>
-      <c r="K192" s="21"/>
-      <c r="L192" s="21"/>
-      <c r="M192" s="21"/>
+      <c r="A192" s="39"/>
+      <c r="B192" s="20"/>
+      <c r="C192" s="24"/>
+      <c r="D192" s="24"/>
+      <c r="E192" s="21"/>
+      <c r="F192" s="21"/>
+      <c r="G192" s="24"/>
+      <c r="H192" s="21"/>
+      <c r="I192" s="21"/>
+      <c r="J192" s="21"/>
+      <c r="K192" s="20"/>
+      <c r="L192" s="20"/>
+      <c r="M192" s="42"/>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A193" s="42"/>
-      <c r="B193" s="21"/>
-      <c r="C193" s="21"/>
-      <c r="D193" s="25"/>
-      <c r="E193" s="22"/>
-      <c r="F193" s="22"/>
-      <c r="G193" s="25"/>
-      <c r="H193" s="22"/>
-      <c r="I193" s="22"/>
-      <c r="J193" s="22"/>
-      <c r="K193" s="21"/>
-      <c r="L193" s="21"/>
-      <c r="M193" s="21"/>
+      <c r="A193" s="39"/>
+      <c r="B193" s="20"/>
+      <c r="C193" s="24"/>
+      <c r="D193" s="24"/>
+      <c r="E193" s="21"/>
+      <c r="F193" s="21"/>
+      <c r="G193" s="24"/>
+      <c r="H193" s="21"/>
+      <c r="I193" s="21"/>
+      <c r="J193" s="21"/>
+      <c r="K193" s="20"/>
+      <c r="L193" s="20"/>
+      <c r="M193" s="42"/>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A194" s="42"/>
-      <c r="B194" s="21"/>
-      <c r="C194" s="21"/>
-      <c r="D194" s="25"/>
-      <c r="E194" s="22"/>
-      <c r="F194" s="22"/>
-      <c r="G194" s="25"/>
-      <c r="H194" s="22"/>
-      <c r="I194" s="22"/>
-      <c r="J194" s="22"/>
-      <c r="K194" s="21"/>
-      <c r="L194" s="21"/>
-      <c r="M194" s="21"/>
+      <c r="A194" s="39"/>
+      <c r="B194" s="20"/>
+      <c r="C194" s="24"/>
+      <c r="D194" s="24"/>
+      <c r="E194" s="21"/>
+      <c r="F194" s="21"/>
+      <c r="G194" s="24"/>
+      <c r="H194" s="21"/>
+      <c r="I194" s="21"/>
+      <c r="J194" s="21"/>
+      <c r="K194" s="20"/>
+      <c r="L194" s="20"/>
+      <c r="M194" s="42"/>
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A195" s="39"/>
-      <c r="B195" s="21"/>
-      <c r="C195" s="21"/>
-      <c r="D195" s="25"/>
-      <c r="E195" s="23"/>
-      <c r="F195" s="23"/>
-      <c r="G195" s="25"/>
-      <c r="H195" s="24"/>
-      <c r="I195" s="24"/>
-      <c r="J195" s="24"/>
-      <c r="K195" s="21"/>
-      <c r="L195" s="21"/>
-      <c r="M195" s="21"/>
+      <c r="A195" s="36"/>
+      <c r="B195" s="20"/>
+      <c r="C195" s="24"/>
+      <c r="D195" s="24"/>
+      <c r="E195" s="22"/>
+      <c r="F195" s="22"/>
+      <c r="G195" s="24"/>
+      <c r="H195" s="23"/>
+      <c r="I195" s="23"/>
+      <c r="J195" s="23"/>
+      <c r="K195" s="20"/>
+      <c r="L195" s="20"/>
+      <c r="M195" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="17">

</xml_diff>

<commit_message>
add to stat_board Hardware&Software
</commit_message>
<xml_diff>
--- a/public/templates/rictu_report_template.xlsx
+++ b/public/templates/rictu_report_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laravel\dilg4a_portal\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40F76D1-DC8E-4AAA-AA17-1982BADCCCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7EC3FF-A809-436B-B5E1-A67F3DFDD747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -581,6 +581,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -610,30 +634,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -974,7 +974,7 @@
   <dimension ref="A1:M195"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="C4" sqref="C4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1012,50 +1012,50 @@
     <row r="2" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
       <c r="H2" s="11"/>
       <c r="I2"/>
       <c r="J2"/>
-      <c r="K2" s="54" t="s">
+      <c r="K2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="55"/>
-      <c r="M2" s="56"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="46"/>
     </row>
     <row r="3" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
       <c r="H3" s="11"/>
       <c r="I3"/>
       <c r="J3"/>
-      <c r="K3" s="57" t="s">
+      <c r="K3" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="58"/>
-      <c r="M3" s="59"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="49"/>
     </row>
     <row r="4" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4"/>
       <c r="B4"/>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4" s="3" t="s">
@@ -1071,12 +1071,12 @@
     <row r="5" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5"/>
       <c r="B5"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5" s="4" t="s">
@@ -1103,70 +1103,70 @@
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
     </row>
     <row r="8" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="46" t="s">
+      <c r="D8" s="57"/>
+      <c r="E8" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="46" t="s">
+      <c r="F8" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="46" t="s">
+      <c r="G8" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="46" t="s">
+      <c r="H8" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="48" t="s">
+      <c r="I8" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="49"/>
-      <c r="K8" s="48" t="s">
+      <c r="J8" s="57"/>
+      <c r="K8" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="49"/>
-      <c r="M8" s="50" t="s">
+      <c r="L8" s="57"/>
+      <c r="M8" s="58" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="47"/>
-      <c r="B9" s="47"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
       <c r="I9" s="12" t="s">
         <v>6</v>
       </c>
@@ -1179,7 +1179,7 @@
       <c r="L9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="51"/>
+      <c r="M9" s="59"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="25"/>
@@ -1838,11 +1838,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="C4:H5"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:M7"/>
     <mergeCell ref="H8:H9"/>
@@ -1855,6 +1850,11 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="C4:H5"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.15748031496062992" bottom="0.23622047244094491" header="0.15748031496062992" footer="0.27559055118110237"/>
   <pageSetup paperSize="9" scale="70" fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>